<commit_message>
customer configuration coding completed. testing in progress.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/process_with_inputs_and_outputs_modify_test_cases.xlsx
+++ b/soberano/test_cases/process_with_inputs_and_outputs_modify_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t xml:space="preserve">Every test case is executed by User1.</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t xml:space="preserve">mm7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mm7 45%, mm8 40%, mm9 15%</t>
   </si>
   <si>
     <t xml:space="preserve">mm5</t>
@@ -452,7 +449,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -865,7 +862,7 @@
         <v>34</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -910,7 +907,7 @@
         <v>50</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>53</v>
@@ -941,7 +938,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -949,7 +946,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -957,7 +954,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,7 +962,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +970,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,7 +978,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -989,7 +986,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -997,7 +994,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,7 +1002,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1010,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1021,7 +1018,7 @@
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,7 +1026,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>